<commit_message>
add start,end date in space,change add in space;delay from XL,child element
</commit_message>
<xml_diff>
--- a/src/main/resources/objectLocator/OR_Common.xlsx
+++ b/src/main/resources/objectLocator/OR_Common.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E410CB-4FE9-4B75-A5EB-7007B05B714C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6BC1D4-3C47-40DF-A245-E276FAB30A8F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RecurringPayment" sheetId="12" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="217">
   <si>
     <t>ObjReference</t>
   </si>
@@ -328,15 +328,9 @@
     <t>startDate</t>
   </si>
   <si>
-    <t>//*[contains(@id,'__START_DATE')]</t>
-  </si>
-  <si>
     <t>endDate</t>
   </si>
   <si>
-    <t>//*[contains(@id,'__END_DATE')]</t>
-  </si>
-  <si>
     <t>btnSave</t>
   </si>
   <si>
@@ -424,9 +418,6 @@
     <t>//*[@id="ddlLeaseTypes_listbox"]</t>
   </si>
   <si>
-    <t>testamt.com/Home/Index</t>
-  </si>
-  <si>
     <t>pgAMTHome</t>
   </si>
   <si>
@@ -665,6 +656,27 @@
   </si>
   <si>
     <t>//*[contains(@id,"_ucPS_pnlContainer")]</t>
+  </si>
+  <si>
+    <t>//*[contains(@aria-owns,"_START_DATE")]</t>
+  </si>
+  <si>
+    <t>//*[contains(@aria-owns,"_END_DATE")]</t>
+  </si>
+  <si>
+    <t>*amt*.com/Home/Index</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>//*[contains(@class,'btnSpaceManagement_DetailAdd')]</t>
+  </si>
+  <si>
+    <t>//*[contains(@id,'grdSpaceManagement')]</t>
+  </si>
+  <si>
+    <t>pnlSpace</t>
   </si>
 </sst>
 </file>
@@ -766,7 +778,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -798,11 +810,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1209,10 +1234,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD51E865-2458-4A55-AA79-2C102593FD0A}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1221,9 +1246,10 @@
     <col min="2" max="2" width="37.85546875" customWidth="1"/>
     <col min="3" max="3" width="48.140625" customWidth="1"/>
     <col min="4" max="4" width="42.7109375" customWidth="1"/>
+    <col min="5" max="5" width="56.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1236,222 +1262,229 @@
       <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>140</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>141</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
         <v>144</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>147</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
         <v>150</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
         <v>153</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>156</v>
-      </c>
-      <c r="D8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
         <v>160</v>
       </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
         <v>161</v>
       </c>
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" t="s">
-        <v>169</v>
-      </c>
       <c r="D16" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A10:A18">
-    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1460,20 +1493,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.42578125" customWidth="1"/>
-    <col min="3" max="3" width="96.28515625" customWidth="1"/>
+    <col min="3" max="3" width="41.28515625" customWidth="1"/>
+    <col min="4" max="4" width="56.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1483,8 +1517,11 @@
       <c r="C1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1494,8 +1531,9 @@
       <c r="C2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1505,8 +1543,9 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1516,8 +1555,9 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1527,13 +1567,14 @@
       <c r="C5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -1541,7 +1582,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1552,7 +1593,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1563,7 +1604,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1574,7 +1615,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1585,7 +1626,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1598,7 +1639,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A8">
-    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1606,10 +1647,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76E70099-CEBC-4B70-8574-EF45A2018E13}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1617,9 +1658,10 @@
     <col min="1" max="1" width="30.85546875" customWidth="1"/>
     <col min="2" max="2" width="29.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="56.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1629,39 +1671,52 @@
       <c r="C1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="10" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="9" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1669,10 +1724,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63457F8-4820-4E80-A0BD-86B1DB623BD5}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1680,9 +1735,10 @@
     <col min="1" max="1" width="59.85546875" customWidth="1"/>
     <col min="2" max="2" width="44.5703125" customWidth="1"/>
     <col min="3" max="3" width="57" customWidth="1"/>
+    <col min="4" max="4" width="56.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1692,8 +1748,11 @@
       <c r="C1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
@@ -1703,8 +1762,9 @@
       <c r="C2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -1714,8 +1774,9 @@
       <c r="C3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -1725,8 +1786,9 @@
       <c r="C4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
@@ -1736,8 +1798,9 @@
       <c r="C5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
@@ -1748,7 +1811,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
@@ -1759,7 +1822,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
@@ -1770,7 +1833,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1781,7 +1844,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1792,7 +1855,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1803,7 +1866,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -1814,9 +1877,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -1825,9 +1888,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
@@ -1836,9 +1899,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
@@ -1847,7 +1910,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -1893,84 +1956,84 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B24" t="s">
         <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B25" t="s">
         <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B26" t="s">
         <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A8">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1979,21 +2042,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC24E92E-F997-460A-B0F8-A599A67DEE36}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="57.140625" customWidth="1"/>
-    <col min="4" max="4" width="56.5703125" customWidth="1"/>
+    <col min="3" max="3" width="97.5703125" customWidth="1"/>
+    <col min="4" max="5" width="56.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2006,8 +2069,11 @@
       <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>90</v>
       </c>
@@ -2020,8 +2086,9 @@
       <c r="D2" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -2032,8 +2099,9 @@
         <v>94</v>
       </c>
       <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>95</v>
       </c>
@@ -2044,8 +2112,9 @@
         <v>96</v>
       </c>
       <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>97</v>
       </c>
@@ -2056,8 +2125,9 @@
         <v>98</v>
       </c>
       <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>99</v>
       </c>
@@ -2065,67 +2135,84 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
         <v>103</v>
       </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>214</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>110</v>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A9 A11">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  <conditionalFormatting sqref="A9 A11:A12">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2134,10 +2221,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F63B57-EF66-439D-B48A-4F7B8AB73CB4}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2145,10 +2232,10 @@
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="64.7109375" customWidth="1"/>
-    <col min="4" max="4" width="56.5703125" customWidth="1"/>
+    <col min="4" max="5" width="56.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2161,8 +2248,11 @@
       <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>59</v>
       </c>
@@ -2175,8 +2265,9 @@
       <c r="D2" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -2187,8 +2278,9 @@
         <v>77</v>
       </c>
       <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>61</v>
       </c>
@@ -2199,8 +2291,9 @@
         <v>80</v>
       </c>
       <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>62</v>
       </c>
@@ -2211,8 +2304,9 @@
         <v>81</v>
       </c>
       <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>56</v>
       </c>
@@ -2226,7 +2320,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>63</v>
       </c>
@@ -2240,7 +2334,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>65</v>
       </c>
@@ -2254,7 +2348,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>67</v>
       </c>
@@ -2265,7 +2359,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -2276,9 +2370,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -2290,7 +2384,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -2301,70 +2395,70 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2375,40 +2469,40 @@
         <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D19" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D20" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2417,10 +2511,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E6D20C-25AD-4167-A7E6-F426B5200648}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2429,9 +2523,10 @@
     <col min="2" max="2" width="37.85546875" customWidth="1"/>
     <col min="3" max="3" width="48.140625" customWidth="1"/>
     <col min="4" max="4" width="42.7109375" customWidth="1"/>
+    <col min="5" max="5" width="56.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2444,8 +2539,11 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -2455,8 +2553,9 @@
       <c r="C2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -2466,20 +2565,22 @@
       <c r="C3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2489,10 +2590,11 @@
       <c r="C5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -2501,132 +2603,132 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>114</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="D9" t="s">
         <v>116</v>
       </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>117</v>
       </c>
-      <c r="D9" t="s">
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D10" t="s">
         <v>119</v>
       </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>120</v>
-      </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>123</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" t="s">
         <v>125</v>
       </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>126</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
         <v>128</v>
       </c>
-      <c r="D13" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="D14" t="s">
         <v>129</v>
       </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" t="s">
-        <v>130</v>
-      </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
         <v>134</v>
       </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="D16" t="s">
         <v>135</v>
-      </c>
-      <c r="D15" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>139</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" t="s">
-        <v>137</v>
-      </c>
-      <c r="D16" t="s">
-        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revision Trigger and Edit revision
</commit_message>
<xml_diff>
--- a/src/main/resources/objectLocator/OR_Common.xlsx
+++ b/src/main/resources/objectLocator/OR_Common.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6BC1D4-3C47-40DF-A245-E276FAB30A8F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7D4C16-0EDF-4FC6-9032-F4E2225C86F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="RecurringPayment" sheetId="12" r:id="rId1"/>
-    <sheet name="Login" sheetId="1" r:id="rId2"/>
-    <sheet name="Homepage" sheetId="11" r:id="rId3"/>
-    <sheet name="Property" sheetId="7" r:id="rId4"/>
-    <sheet name="Space" sheetId="10" r:id="rId5"/>
-    <sheet name="Lease" sheetId="8" r:id="rId6"/>
-    <sheet name="GlobalSearch" sheetId="9" r:id="rId7"/>
+    <sheet name="ClientProfile" sheetId="13" r:id="rId1"/>
+    <sheet name="RecurringPayment" sheetId="12" r:id="rId2"/>
+    <sheet name="Login" sheetId="1" r:id="rId3"/>
+    <sheet name="Homepage" sheetId="11" r:id="rId4"/>
+    <sheet name="Property" sheetId="7" r:id="rId5"/>
+    <sheet name="Space" sheetId="10" r:id="rId6"/>
+    <sheet name="Lease" sheetId="8" r:id="rId7"/>
+    <sheet name="GlobalSearch" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="221">
   <si>
     <t>ObjReference</t>
   </si>
@@ -677,6 +678,18 @@
   </si>
   <si>
     <t>pnlSpace</t>
+  </si>
+  <si>
+    <t>//*[contains(@id,"FMV_Of_Lease")]</t>
+  </si>
+  <si>
+    <t>//*[contains(@id,"Useful_Life")]</t>
+  </si>
+  <si>
+    <t>txtUsefulLife</t>
+  </si>
+  <si>
+    <t>txtFMVOfLease</t>
   </si>
 </sst>
 </file>
@@ -1233,11 +1246,73 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D8BA34-2166-435E-930D-384774C7AB09}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" customWidth="1"/>
+    <col min="5" max="5" width="56.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD51E865-2458-4A55-AA79-2C102593FD0A}">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1491,7 +1566,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -1645,7 +1720,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76E70099-CEBC-4B70-8574-EF45A2018E13}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -1722,7 +1797,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63457F8-4820-4E80-A0BD-86B1DB623BD5}">
   <dimension ref="A1:D26"/>
   <sheetViews>
@@ -2040,12 +2115,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC24E92E-F997-460A-B0F8-A599A67DEE36}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2212,14 +2287,14 @@
     <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F63B57-EF66-439D-B48A-4F7B8AB73CB4}">
   <dimension ref="A1:E21"/>
   <sheetViews>
@@ -2502,14 +2577,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E6D20C-25AD-4167-A7E6-F426B5200648}">
   <dimension ref="A1:E16"/>
   <sheetViews>

</xml_diff>

<commit_message>
Add: Login test case for different browser and Some methods in keywordscript
</commit_message>
<xml_diff>
--- a/src/main/resources/objectLocator/OR_Common.xlsx
+++ b/src/main/resources/objectLocator/OR_Common.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7D4C16-0EDF-4FC6-9032-F4E2225C86F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="780" windowWidth="20730" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ClientProfile" sheetId="13" r:id="rId1"/>
@@ -17,7 +16,7 @@
     <sheet name="Lease" sheetId="8" r:id="rId7"/>
     <sheet name="GlobalSearch" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="225">
   <si>
     <t>ObjReference</t>
   </si>
@@ -690,12 +689,24 @@
   </si>
   <si>
     <t>txtFMVOfLease</t>
+  </si>
+  <si>
+    <t>pgAMTAppLogin</t>
+  </si>
+  <si>
+    <t>app.amtdirect.com</t>
+  </si>
+  <si>
+    <t>//*[@id='module-bar']</t>
+  </si>
+  <si>
+    <t>navDashboard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1246,10 +1257,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D8BA34-2166-435E-930D-384774C7AB09}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1308,7 +1319,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD51E865-2458-4A55-AA79-2C102593FD0A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1567,11 +1578,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1712,16 +1723,36 @@
         <v>23</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>221</v>
+      </c>
+      <c r="C13" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>223</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A8">
     <cfRule type="duplicateValues" dxfId="12" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76E70099-CEBC-4B70-8574-EF45A2018E13}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1798,7 +1829,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63457F8-4820-4E80-A0BD-86B1DB623BD5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2116,7 +2147,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC24E92E-F997-460A-B0F8-A599A67DEE36}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2295,7 +2326,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F63B57-EF66-439D-B48A-4F7B8AB73CB4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2585,7 +2616,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E6D20C-25AD-4167-A7E6-F426B5200648}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Data Create + OR + Module Controller .XLSX file Added
</commit_message>
<xml_diff>
--- a/src/main/resources/objectLocator/OR_Common.xlsx
+++ b/src/main/resources/objectLocator/OR_Common.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83A95FF-319E-B24B-A32A-D810139CB67A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="3930" windowWidth="20730" windowHeight="10305" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ClientProfile" sheetId="13" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="244">
   <si>
     <t>ObjReference</t>
   </si>
@@ -746,13 +747,25 @@
   </si>
   <si>
     <t>txtFiscalYear</t>
+  </si>
+  <si>
+    <t>fiscalYear</t>
+  </si>
+  <si>
+    <t>//*[contains(@id,'__fiscal_year')]</t>
+  </si>
+  <si>
+    <t>fiscalYearByAreaOwns</t>
+  </si>
+  <si>
+    <t>//*[contains(@aria-controls,'__fiscal_year_dateview')]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -799,6 +812,12 @@
       <color rgb="FF6A8759"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -853,7 +872,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -891,6 +910,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1311,23 +1331,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1"/>
-    <col min="2" max="2" width="37.85546875" customWidth="1"/>
-    <col min="3" max="3" width="48.140625" customWidth="1"/>
-    <col min="4" max="4" width="42.7109375" customWidth="1"/>
-    <col min="5" max="5" width="56.5703125" customWidth="1"/>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="37.83203125" customWidth="1"/>
+    <col min="3" max="3" width="48.1640625" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" customWidth="1"/>
+    <col min="5" max="5" width="56.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1344,7 +1364,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>220</v>
       </c>
@@ -1355,7 +1375,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>219</v>
       </c>
@@ -1373,23 +1393,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1"/>
-    <col min="2" max="2" width="37.85546875" customWidth="1"/>
-    <col min="3" max="3" width="48.140625" customWidth="1"/>
-    <col min="4" max="4" width="42.7109375" customWidth="1"/>
-    <col min="5" max="5" width="56.5703125" customWidth="1"/>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="37.83203125" customWidth="1"/>
+    <col min="3" max="3" width="48.1640625" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" customWidth="1"/>
+    <col min="5" max="5" width="56.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1406,7 +1426,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>173</v>
       </c>
@@ -1421,7 +1441,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>137</v>
       </c>
@@ -1436,7 +1456,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>140</v>
       </c>
@@ -1451,7 +1471,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>143</v>
       </c>
@@ -1466,7 +1486,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>146</v>
       </c>
@@ -1480,7 +1500,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>149</v>
       </c>
@@ -1494,7 +1514,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>152</v>
       </c>
@@ -1508,7 +1528,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>101</v>
       </c>
@@ -1519,7 +1539,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>102</v>
       </c>
@@ -1530,7 +1550,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>157</v>
       </c>
@@ -1542,7 +1562,7 @@
       </c>
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>159</v>
       </c>
@@ -1553,7 +1573,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>100</v>
       </c>
@@ -1564,7 +1584,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>162</v>
       </c>
@@ -1575,7 +1595,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>164</v>
       </c>
@@ -1586,7 +1606,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>165</v>
       </c>
@@ -1600,7 +1620,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>167</v>
       </c>
@@ -1611,7 +1631,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>169</v>
       </c>
@@ -1622,7 +1642,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>190</v>
       </c>
@@ -1633,7 +1653,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>231</v>
       </c>
@@ -1645,7 +1665,7 @@
       </c>
       <c r="D20" s="9"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>232</v>
       </c>
@@ -1656,7 +1676,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>233</v>
       </c>
@@ -1667,7 +1687,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>235</v>
       </c>
@@ -1678,7 +1698,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>237</v>
       </c>
@@ -1689,7 +1709,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>239</v>
       </c>
@@ -1698,6 +1718,28 @@
       </c>
       <c r="C25" t="s">
         <v>238</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -1710,22 +1752,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" customWidth="1"/>
-    <col min="4" max="4" width="56.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5" customWidth="1"/>
+    <col min="3" max="3" width="41.33203125" customWidth="1"/>
+    <col min="4" max="4" width="56.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1739,7 +1781,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1751,7 +1793,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1763,7 +1805,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1775,7 +1817,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1787,12 +1829,12 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -1800,7 +1842,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1811,7 +1853,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1822,7 +1864,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1833,7 +1875,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1844,7 +1886,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1855,7 +1897,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>221</v>
       </c>
@@ -1863,7 +1905,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>224</v>
       </c>
@@ -1874,7 +1916,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>226</v>
       </c>
@@ -1885,7 +1927,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>227</v>
       </c>
@@ -1906,22 +1948,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="56.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="56.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1935,7 +1977,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>130</v>
       </c>
@@ -1944,13 +1986,13 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D5" s="1"/>
     </row>
   </sheetData>
@@ -1983,22 +2025,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="59.85546875" customWidth="1"/>
-    <col min="2" max="2" width="44.5703125" customWidth="1"/>
+    <col min="1" max="1" width="59.83203125" customWidth="1"/>
+    <col min="2" max="2" width="44.5" customWidth="1"/>
     <col min="3" max="3" width="57" customWidth="1"/>
-    <col min="4" max="4" width="56.5703125" customWidth="1"/>
+    <col min="4" max="4" width="56.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2012,7 +2054,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
@@ -2024,7 +2066,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -2036,7 +2078,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -2048,7 +2090,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
@@ -2060,7 +2102,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
@@ -2071,7 +2113,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
@@ -2082,7 +2124,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
@@ -2093,7 +2135,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -2104,7 +2146,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -2115,7 +2157,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -2126,7 +2168,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -2137,7 +2179,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>177</v>
       </c>
@@ -2148,7 +2190,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>178</v>
       </c>
@@ -2159,7 +2201,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>179</v>
       </c>
@@ -2170,7 +2212,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -2181,7 +2223,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -2192,7 +2234,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -2203,7 +2245,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -2214,7 +2256,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>176</v>
       </c>
@@ -2225,7 +2267,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>181</v>
       </c>
@@ -2236,7 +2278,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>187</v>
       </c>
@@ -2247,7 +2289,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>189</v>
       </c>
@@ -2258,7 +2300,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>203</v>
       </c>
@@ -2269,7 +2311,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>206</v>
       </c>
@@ -2280,7 +2322,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>208</v>
       </c>
@@ -2301,22 +2343,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="97.5703125" customWidth="1"/>
-    <col min="4" max="5" width="56.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="97.5" customWidth="1"/>
+    <col min="4" max="5" width="56.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2333,7 +2375,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>90</v>
       </c>
@@ -2348,7 +2390,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -2361,7 +2403,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>95</v>
       </c>
@@ -2374,7 +2416,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>97</v>
       </c>
@@ -2387,7 +2429,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>99</v>
       </c>
@@ -2398,7 +2440,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>100</v>
       </c>
@@ -2409,7 +2451,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>101</v>
       </c>
@@ -2420,7 +2462,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>102</v>
       </c>
@@ -2431,7 +2473,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>104</v>
       </c>
@@ -2445,7 +2487,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>109</v>
       </c>
@@ -2456,7 +2498,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>216</v>
       </c>
@@ -2480,22 +2522,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="64.7109375" customWidth="1"/>
-    <col min="4" max="5" width="56.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="64.6640625" customWidth="1"/>
+    <col min="4" max="5" width="56.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2512,7 +2554,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>59</v>
       </c>
@@ -2527,7 +2569,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -2540,7 +2582,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>61</v>
       </c>
@@ -2553,7 +2595,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>62</v>
       </c>
@@ -2566,7 +2608,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>56</v>
       </c>
@@ -2580,7 +2622,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>63</v>
       </c>
@@ -2594,7 +2636,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>65</v>
       </c>
@@ -2608,7 +2650,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>67</v>
       </c>
@@ -2619,7 +2661,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -2630,7 +2672,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>180</v>
       </c>
@@ -2644,7 +2686,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -2655,7 +2697,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>104</v>
       </c>
@@ -2666,7 +2708,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>171</v>
       </c>
@@ -2677,7 +2719,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>184</v>
       </c>
@@ -2688,7 +2730,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>185</v>
       </c>
@@ -2699,7 +2741,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>194</v>
       </c>
@@ -2710,7 +2752,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>189</v>
       </c>
@@ -2721,7 +2763,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -2735,7 +2777,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>114</v>
       </c>
@@ -2749,7 +2791,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>201</v>
       </c>
@@ -2770,23 +2812,23 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1"/>
-    <col min="2" max="2" width="37.85546875" customWidth="1"/>
-    <col min="3" max="3" width="48.140625" customWidth="1"/>
-    <col min="4" max="4" width="42.7109375" customWidth="1"/>
-    <col min="5" max="5" width="56.5703125" customWidth="1"/>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="37.83203125" customWidth="1"/>
+    <col min="3" max="3" width="48.1640625" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" customWidth="1"/>
+    <col min="5" max="5" width="56.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2803,7 +2845,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -2815,7 +2857,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -2827,7 +2869,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -2840,7 +2882,7 @@
       <c r="D4" s="9"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2852,7 +2894,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>107</v>
       </c>
@@ -2863,7 +2905,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>111</v>
       </c>
@@ -2874,7 +2916,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>112</v>
       </c>
@@ -2885,7 +2927,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -2899,7 +2941,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>117</v>
       </c>
@@ -2913,7 +2955,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>121</v>
       </c>
@@ -2924,7 +2966,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>123</v>
       </c>
@@ -2935,7 +2977,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>124</v>
       </c>
@@ -2949,7 +2991,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>127</v>
       </c>
@@ -2963,7 +3005,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>131</v>
       </c>
@@ -2977,7 +3019,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>136</v>
       </c>

</xml_diff>

<commit_message>
Partial commit of second revision
</commit_message>
<xml_diff>
--- a/src/main/resources/objectLocator/OR_Common.xlsx
+++ b/src/main/resources/objectLocator/OR_Common.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83A95FF-319E-B24B-A32A-D810139CB67A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="33600" windowHeight="21000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ClientProfile" sheetId="13" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="247">
   <si>
     <t>ObjReference</t>
   </si>
@@ -759,13 +758,22 @@
   </si>
   <si>
     <t>//*[contains(@aria-controls,'__fiscal_year_dateview')]</t>
+  </si>
+  <si>
+    <t>btnEdit</t>
+  </si>
+  <si>
+    <t>//input[contains(@id,'vamount')]/preceding-sibling::input</t>
+  </si>
+  <si>
+    <t>txtRprAmount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1331,23 +1339,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.5" customWidth="1"/>
-    <col min="2" max="2" width="37.83203125" customWidth="1"/>
-    <col min="3" max="3" width="48.1640625" customWidth="1"/>
-    <col min="4" max="4" width="42.6640625" customWidth="1"/>
-    <col min="5" max="5" width="56.5" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" customWidth="1"/>
+    <col min="5" max="5" width="56.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1364,7 +1372,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>220</v>
       </c>
@@ -1375,7 +1383,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>219</v>
       </c>
@@ -1393,23 +1401,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.5" customWidth="1"/>
-    <col min="2" max="2" width="37.83203125" customWidth="1"/>
-    <col min="3" max="3" width="48.1640625" customWidth="1"/>
-    <col min="4" max="4" width="42.6640625" customWidth="1"/>
-    <col min="5" max="5" width="56.5" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" customWidth="1"/>
+    <col min="3" max="3" width="66.28515625" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" customWidth="1"/>
+    <col min="5" max="5" width="56.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1426,7 +1434,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="5" t="s">
         <v>173</v>
       </c>
@@ -1441,7 +1449,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
         <v>137</v>
       </c>
@@ -1456,7 +1464,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>140</v>
       </c>
@@ -1471,7 +1479,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" s="3" t="s">
         <v>143</v>
       </c>
@@ -1486,7 +1494,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
         <v>146</v>
       </c>
@@ -1500,7 +1508,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
         <v>149</v>
       </c>
@@ -1514,7 +1522,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
         <v>152</v>
       </c>
@@ -1528,7 +1536,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15.75" thickBot="1">
       <c r="A9" s="7" t="s">
         <v>101</v>
       </c>
@@ -1539,7 +1547,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
         <v>102</v>
       </c>
@@ -1550,7 +1558,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" s="8" t="s">
         <v>157</v>
       </c>
@@ -1562,7 +1570,7 @@
       </c>
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" s="8" t="s">
         <v>159</v>
       </c>
@@ -1573,7 +1581,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" s="8" t="s">
         <v>100</v>
       </c>
@@ -1584,7 +1592,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" s="8" t="s">
         <v>162</v>
       </c>
@@ -1595,7 +1603,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" s="8" t="s">
         <v>164</v>
       </c>
@@ -1606,7 +1614,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" s="8" t="s">
         <v>165</v>
       </c>
@@ -1620,7 +1628,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" s="8" t="s">
         <v>167</v>
       </c>
@@ -1631,7 +1639,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" s="8" t="s">
         <v>169</v>
       </c>
@@ -1642,7 +1650,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" s="8" t="s">
         <v>190</v>
       </c>
@@ -1653,7 +1661,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>231</v>
       </c>
@@ -1665,7 +1673,7 @@
       </c>
       <c r="D20" s="9"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" s="9" t="s">
         <v>232</v>
       </c>
@@ -1676,7 +1684,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" s="9" t="s">
         <v>233</v>
       </c>
@@ -1687,7 +1695,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>235</v>
       </c>
@@ -1698,7 +1706,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>237</v>
       </c>
@@ -1709,7 +1717,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>239</v>
       </c>
@@ -1720,7 +1728,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" s="15" t="s">
         <v>240</v>
       </c>
@@ -1731,7 +1739,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" s="15" t="s">
         <v>242</v>
       </c>
@@ -1740,6 +1748,28 @@
       </c>
       <c r="C27" t="s">
         <v>243</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>246</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -1752,22 +1782,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.5" customWidth="1"/>
-    <col min="3" max="3" width="41.33203125" customWidth="1"/>
-    <col min="4" max="4" width="56.5" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" customWidth="1"/>
+    <col min="3" max="3" width="41.28515625" customWidth="1"/>
+    <col min="4" max="4" width="56.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1781,7 +1811,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1793,7 +1823,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1805,7 +1835,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1817,7 +1847,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1829,12 +1859,12 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15.75" thickBot="1">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -1842,7 +1872,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1853,7 +1883,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1864,7 +1894,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1875,7 +1905,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1886,7 +1916,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1897,7 +1927,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>221</v>
       </c>
@@ -1905,7 +1935,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" s="9" t="s">
         <v>224</v>
       </c>
@@ -1916,7 +1946,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>226</v>
       </c>
@@ -1927,7 +1957,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>227</v>
       </c>
@@ -1948,22 +1978,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.83203125" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" customWidth="1"/>
-    <col min="4" max="4" width="56.5" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="56.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1977,7 +2007,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="10" t="s">
         <v>130</v>
       </c>
@@ -1986,13 +2016,13 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="D5" s="1"/>
     </row>
   </sheetData>
@@ -2025,22 +2055,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="59.83203125" customWidth="1"/>
-    <col min="2" max="2" width="44.5" customWidth="1"/>
+    <col min="1" max="1" width="59.85546875" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" customWidth="1"/>
     <col min="3" max="3" width="57" customWidth="1"/>
-    <col min="4" max="4" width="56.5" customWidth="1"/>
+    <col min="4" max="4" width="56.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2054,7 +2084,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
@@ -2066,7 +2096,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -2078,7 +2108,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -2090,7 +2120,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
@@ -2102,7 +2132,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
@@ -2113,7 +2143,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15.75" thickBot="1">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
@@ -2124,7 +2154,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
@@ -2135,7 +2165,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -2146,7 +2176,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -2157,7 +2187,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -2168,7 +2198,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -2179,7 +2209,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>177</v>
       </c>
@@ -2190,7 +2220,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>178</v>
       </c>
@@ -2201,7 +2231,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>179</v>
       </c>
@@ -2212,7 +2242,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -2223,7 +2253,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -2234,7 +2264,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -2245,7 +2275,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -2256,7 +2286,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>176</v>
       </c>
@@ -2267,7 +2297,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>181</v>
       </c>
@@ -2278,7 +2308,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>187</v>
       </c>
@@ -2289,7 +2319,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>189</v>
       </c>
@@ -2300,7 +2330,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>203</v>
       </c>
@@ -2311,7 +2341,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>206</v>
       </c>
@@ -2322,7 +2352,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>208</v>
       </c>
@@ -2343,22 +2373,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="97.5" customWidth="1"/>
-    <col min="4" max="5" width="56.5" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="97.42578125" customWidth="1"/>
+    <col min="4" max="5" width="56.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2375,7 +2405,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
         <v>90</v>
       </c>
@@ -2390,7 +2420,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -2403,7 +2433,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
         <v>95</v>
       </c>
@@ -2416,7 +2446,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" s="3" t="s">
         <v>97</v>
       </c>
@@ -2429,7 +2459,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
         <v>99</v>
       </c>
@@ -2440,7 +2470,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
         <v>100</v>
       </c>
@@ -2451,7 +2481,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1">
       <c r="A8" s="7" t="s">
         <v>101</v>
       </c>
@@ -2462,7 +2492,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
         <v>102</v>
       </c>
@@ -2473,7 +2503,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>104</v>
       </c>
@@ -2487,7 +2517,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" s="8" t="s">
         <v>109</v>
       </c>
@@ -2498,7 +2528,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" s="13" t="s">
         <v>216</v>
       </c>
@@ -2522,22 +2552,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="64.6640625" customWidth="1"/>
-    <col min="4" max="5" width="56.5" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="64.7109375" customWidth="1"/>
+    <col min="4" max="5" width="56.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2554,7 +2584,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
         <v>59</v>
       </c>
@@ -2569,7 +2599,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -2582,7 +2612,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
         <v>61</v>
       </c>
@@ -2595,7 +2625,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" s="3" t="s">
         <v>62</v>
       </c>
@@ -2608,7 +2638,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
         <v>56</v>
       </c>
@@ -2622,7 +2652,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
         <v>63</v>
       </c>
@@ -2636,7 +2666,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1">
       <c r="A8" s="7" t="s">
         <v>65</v>
       </c>
@@ -2650,7 +2680,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
         <v>67</v>
       </c>
@@ -2661,7 +2691,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -2672,7 +2702,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>180</v>
       </c>
@@ -2686,7 +2716,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -2697,7 +2727,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>104</v>
       </c>
@@ -2708,7 +2738,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>171</v>
       </c>
@@ -2719,7 +2749,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>184</v>
       </c>
@@ -2730,7 +2760,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>185</v>
       </c>
@@ -2741,7 +2771,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>194</v>
       </c>
@@ -2752,7 +2782,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>189</v>
       </c>
@@ -2763,7 +2793,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -2777,7 +2807,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>114</v>
       </c>
@@ -2791,7 +2821,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>201</v>
       </c>
@@ -2812,23 +2842,23 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.5" customWidth="1"/>
-    <col min="2" max="2" width="37.83203125" customWidth="1"/>
-    <col min="3" max="3" width="48.1640625" customWidth="1"/>
-    <col min="4" max="4" width="42.6640625" customWidth="1"/>
-    <col min="5" max="5" width="56.5" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" customWidth="1"/>
+    <col min="5" max="5" width="56.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2845,7 +2875,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -2857,7 +2887,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -2869,7 +2899,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -2882,7 +2912,7 @@
       <c r="D4" s="9"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2894,7 +2924,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>107</v>
       </c>
@@ -2905,7 +2935,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>111</v>
       </c>
@@ -2916,7 +2946,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>112</v>
       </c>
@@ -2927,7 +2957,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -2941,7 +2971,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>117</v>
       </c>
@@ -2955,7 +2985,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>121</v>
       </c>
@@ -2966,7 +2996,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>123</v>
       </c>
@@ -2977,7 +3007,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>124</v>
       </c>
@@ -2991,7 +3021,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>127</v>
       </c>
@@ -3005,7 +3035,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>131</v>
       </c>
@@ -3019,7 +3049,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>136</v>
       </c>

</xml_diff>

<commit_message>
Fix fiscal year and autopopulate rpr issue. Add: 1. Uibase methods 2.Test cases for SRAT
</commit_message>
<xml_diff>
--- a/src/main/resources/objectLocator/OR_Common.xlsx
+++ b/src/main/resources/objectLocator/OR_Common.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="33600" windowHeight="21000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2250" windowWidth="33600" windowHeight="21000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ClientProfile" sheetId="13" r:id="rId1"/>
@@ -1486,7 +1486,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>

</xml_diff>